<commit_message>
Basic GUI almost completed.
Making all classes with methods V2.4.

 ^Jan for you ;)
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -2,16 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
     <sheet name="CPU" sheetId="2" r:id="rId2"/>
     <sheet name="RAM" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
-  <si>
-    <t>groupComponent</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>nameComponent</t>
   </si>
@@ -50,9 +47,6 @@
     <t>amountGB</t>
   </si>
   <si>
-    <t>Motherboard</t>
-  </si>
-  <si>
     <t>GA-Z87-HD3</t>
   </si>
   <si>
@@ -102,12 +96,39 @@
   </si>
   <si>
     <t>DDR4</t>
+  </si>
+  <si>
+    <t>i7 4770K</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>X4 640</t>
+  </si>
+  <si>
+    <t>AM3</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,12 +165,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,20 +449,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="8" width="16.7109375" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,62 +479,56 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>64</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -522,10 +538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,30 +553,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -572,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -586,36 +630,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>8</v>

</xml_diff>

<commit_message>
Version I dont care
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
     <sheet name="CPU" sheetId="2" r:id="rId2"/>
     <sheet name="RAM" sheetId="3" r:id="rId3"/>
+    <sheet name="GPU" sheetId="4" r:id="rId4"/>
+    <sheet name="PSU" sheetId="5" r:id="rId5"/>
+    <sheet name="Drive" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>nameComponent</t>
   </si>
@@ -123,6 +126,81 @@
   </si>
   <si>
     <t>32</t>
+  </si>
+  <si>
+    <t>GTX 980</t>
+  </si>
+  <si>
+    <t>maxWattage</t>
+  </si>
+  <si>
+    <t>4 GB GDDR5</t>
+  </si>
+  <si>
+    <t>Fury X</t>
+  </si>
+  <si>
+    <t>Nvidia</t>
+  </si>
+  <si>
+    <t>GS800</t>
+  </si>
+  <si>
+    <t>800 Watt</t>
+  </si>
+  <si>
+    <t>Non-modular</t>
+  </si>
+  <si>
+    <t>G550M</t>
+  </si>
+  <si>
+    <t>Cooler Master</t>
+  </si>
+  <si>
+    <t>Semi-Modular</t>
+  </si>
+  <si>
+    <t>550 Watt</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">950 EVO </t>
+  </si>
+  <si>
+    <t>Western Digital</t>
+  </si>
+  <si>
+    <t>WD40EFRX</t>
+  </si>
+  <si>
+    <t>512 GB SDD</t>
+  </si>
+  <si>
+    <t>4 TB HDD</t>
+  </si>
+  <si>
+    <t>Kingston</t>
+  </si>
+  <si>
+    <t>HyperX Fury</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2133 MHz</t>
+  </si>
+  <si>
+    <t>Mother</t>
   </si>
 </sst>
 </file>
@@ -449,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +607,11 @@
       </c>
       <c r="G3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -614,10 +697,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,15 +744,201 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Reading components from an Excel file, done. Making the appropriate objects and putting them in a ArrayList, done. Simple way to get the individual information, kinda done.
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -89,15 +89,9 @@
     <t>maxRAMGB</t>
   </si>
   <si>
-    <t>sdvtervth</t>
-  </si>
-  <si>
     <t>AsRock</t>
   </si>
   <si>
-    <t>dgsgdfgf</t>
-  </si>
-  <si>
     <t>DDR4</t>
   </si>
   <si>
@@ -198,12 +192,18 @@
   </si>
   <si>
     <t>2133 MHz</t>
+  </si>
+  <si>
+    <t>X99 Rampage V Extreme</t>
+  </si>
+  <si>
+    <t>Extended ATX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -527,12 +527,13 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="7" width="16.7109375" customWidth="1"/>
   </cols>
@@ -574,10 +575,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -585,25 +586,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -656,7 +657,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -670,16 +671,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -737,30 +738,30 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -796,24 +797,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -847,35 +848,35 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -910,24 +911,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
We have our first ActionListener!!
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="117">
   <si>
     <t>nameComponent</t>
   </si>
@@ -333,12 +333,54 @@
   </si>
   <si>
     <t>Laptop Hybrid HDD</t>
+  </si>
+  <si>
+    <t>wattUsage</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>wattUsage(/stick)</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>275</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,7 +430,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -666,21 +708,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="7" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,133 +731,151 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
         <v>57</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
         <v>65</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -825,20 +886,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="7" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -846,79 +908,97 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
         <v>67</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -929,21 +1009,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -951,115 +1031,133 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
         <v>72</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>74</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1071,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,9 +1180,10 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1092,61 +1191,79 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1160,7 +1277,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,6 +1285,7 @@
     <col min="1" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1261,20 +1379,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1282,61 +1400,79 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>98</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
       <c r="B6" t="s">
         <v>98</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
userCfg gedeeltelijk klaar selecting component groups werkt ...
-Jan
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,16 +391,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF424242"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF424242"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -423,11 +416,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +703,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +748,7 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D2" t="s">
@@ -765,10 +757,10 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H2" t="s">
@@ -782,7 +774,7 @@
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D3" t="s">
@@ -791,10 +783,10 @@
       <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H3" t="s">
@@ -808,7 +800,7 @@
       <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D4" t="s">
@@ -817,10 +809,10 @@
       <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H4" t="s">
@@ -834,7 +826,7 @@
       <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D5" t="s">
@@ -843,10 +835,10 @@
       <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H5" t="s">
@@ -860,7 +852,7 @@
       <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D6" t="s">
@@ -869,10 +861,10 @@
       <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H6" t="s">
@@ -889,7 +881,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +916,7 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D2" t="s">
@@ -941,7 +933,7 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D3" t="s">
@@ -958,7 +950,7 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D4" t="s">
@@ -975,7 +967,7 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D5" t="s">
@@ -992,7 +984,7 @@
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D6" t="s">
@@ -1012,7 +1004,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,13 +1039,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>110</v>
       </c>
       <c r="D2" t="s">
@@ -1062,10 +1054,10 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1076,7 +1068,7 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D3" t="s">
@@ -1085,10 +1077,10 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1099,7 +1091,7 @@
       <c r="B4" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>110</v>
       </c>
       <c r="D4" t="s">
@@ -1108,10 +1100,10 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1122,7 +1114,7 @@
       <c r="B5" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D5" t="s">
@@ -1131,21 +1123,21 @@
       <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>110</v>
       </c>
       <c r="D6" t="s">
@@ -1154,10 +1146,10 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1171,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1196,7 @@
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>111</v>
       </c>
       <c r="D2" t="s">
@@ -1218,7 +1210,7 @@
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D3" t="s">
@@ -1232,7 +1224,7 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D4" t="s">
@@ -1246,7 +1238,7 @@
       <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D5" t="s">
@@ -1260,7 +1252,7 @@
       <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D6" t="s">
@@ -1381,7 +1373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1413,7 +1405,7 @@
       <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D2" t="s">
@@ -1427,7 +1419,7 @@
       <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D3" t="s">
@@ -1441,7 +1433,7 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D4" t="s">
@@ -1455,7 +1447,7 @@
       <c r="B5" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D5" t="s">
@@ -1469,7 +1461,7 @@
       <c r="B6" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D6" t="s">

</xml_diff>

<commit_message>
TO DO: -search/sort combination => add component
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
@@ -197,9 +197,6 @@
     <t>Intel Graphics 4600, 4 cores</t>
   </si>
   <si>
-    <t>i7 -5960X</t>
-  </si>
-  <si>
     <t>LGA 2011-3</t>
   </si>
   <si>
@@ -375,6 +372,9 @@
   </si>
   <si>
     <t>1.5</t>
+  </si>
+  <si>
+    <t>i7 5960X</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -749,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -775,7 +775,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
@@ -795,19 +795,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>24</v>
@@ -827,7 +827,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
         <v>55</v>
@@ -847,19 +847,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>24</v>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -917,7 +917,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -934,7 +934,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
         <v>56</v>
@@ -945,53 +945,53 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1003,7 +1003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1023,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1046,7 +1046,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -1069,7 +1069,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -1086,16 +1086,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
         <v>69</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1109,16 +1109,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
         <v>71</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" t="s">
-        <v>73</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -1132,16 +1132,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
         <v>74</v>
       </c>
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1197,7 +1197,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -1211,7 +1211,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -1219,44 +1219,44 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1302,10 +1302,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
@@ -1324,27 +1324,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
         <v>83</v>
-      </c>
-      <c r="B4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -1352,16 +1352,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1406,10 +1406,10 @@
         <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>40</v>
@@ -1428,44 +1428,44 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TODO: 1. autosave user cfg when exiting application 2. verification text boxes replaced by only 1 (String input like error box) 3. adding clear button to compare tab 4. cleaning A LOT OF CODE including warnings.
            -Jan
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t xml:space="preserve">950 EVO </t>
-  </si>
-  <si>
     <t>Western Digital</t>
   </si>
   <si>
@@ -375,6 +372,9 @@
   </si>
   <si>
     <t>i7 5960X</t>
+  </si>
+  <si>
+    <t>950 EVO</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -749,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -769,22 +769,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>25</v>
@@ -795,19 +795,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
         <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>24</v>
@@ -821,19 +821,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
         <v>52</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
-        <v>53</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
@@ -847,19 +847,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" t="s">
-        <v>62</v>
-      </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>24</v>
@@ -880,7 +880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -900,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -917,10 +917,10 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -934,10 +934,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -945,53 +945,53 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1046,7 +1046,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -1055,102 +1055,102 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" t="s">
         <v>68</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
         <v>70</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
         <v>71</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
         <v>73</v>
       </c>
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1163,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1197,7 +1197,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -1211,7 +1211,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -1219,44 +1219,44 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1269,7 +1269,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,10 +1302,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
@@ -1324,27 +1324,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -1352,16 +1352,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1374,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1400,72 +1400,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s">
         <v>92</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Variabele componenten in excel kunnen inlezen 2. Cleaning
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
@@ -191,9 +191,6 @@
     <t>ATX,3x PCIe x16</t>
   </si>
   <si>
-    <t>Intel Graphics 4600, 4 cores</t>
-  </si>
-  <si>
     <t>LGA 2011-3</t>
   </si>
   <si>
@@ -375,12 +372,15 @@
   </si>
   <si>
     <t>950 EVO</t>
+  </si>
+  <si>
+    <t>iGPU 4600, 4 cores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,7 +422,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -749,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -775,7 +775,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
@@ -795,19 +795,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>24</v>
@@ -827,7 +827,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -847,19 +847,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>24</v>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -917,10 +917,10 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -934,10 +934,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -945,53 +945,53 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1046,7 +1046,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -1069,7 +1069,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -1086,16 +1086,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" t="s">
         <v>67</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1109,16 +1109,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s">
         <v>70</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" t="s">
-        <v>71</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -1132,16 +1132,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
         <v>72</v>
       </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1163,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1197,7 +1197,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -1211,7 +1211,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -1219,44 +1219,44 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1302,10 +1302,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
@@ -1324,27 +1324,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -1352,16 +1352,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1400,16 +1400,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
@@ -1428,44 +1428,44 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
         <v>91</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Cleaning code 2. Boolean voor calculate watt zie mateusz offerfile 3. Delete popup
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="116">
   <si>
     <t>nameComponent</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>ATX,3x PCIe x16</t>
-  </si>
-  <si>
-    <t>LGA 2011-3</t>
   </si>
   <si>
     <t>8 cores, 3 GHz</t>
@@ -723,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -749,7 +746,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -775,7 +772,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
@@ -795,19 +792,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>24</v>
@@ -827,7 +824,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -847,19 +844,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>24</v>
@@ -881,7 +878,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -917,10 +914,10 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -934,10 +931,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -945,53 +942,53 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1046,7 +1043,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -1069,7 +1066,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -1086,16 +1083,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
         <v>65</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
         <v>66</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1109,16 +1106,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" t="s">
         <v>69</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -1132,16 +1129,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>71</v>
       </c>
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1183,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1197,7 +1194,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -1211,7 +1208,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -1219,44 +1216,44 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1302,10 +1299,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1316,7 +1313,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
@@ -1324,27 +1321,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
         <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -1352,16 +1349,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1400,16 +1397,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1417,7 @@
         <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
@@ -1428,44 +1425,44 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" t="s">
         <v>90</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>